<commit_message>
Fleshed out various things about the FileSheet and added a settings import from serialized xml.
</commit_message>
<xml_diff>
--- a/HelloWorld/Template.xlsx
+++ b/HelloWorld/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grins\source\repos\HelloWorld\HelloWorld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA4E99E-214B-45A7-BEA9-1489DB57F20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28190DC-6679-4F48-8EF5-5D013FE1C9E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2F07DCDD-1F4C-4582-9DE4-20C2F28E34DC}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>Options</t>
   </si>
   <si>
-    <t>C:\Users\grins\source\repos\HelloWorld\HelloWorld\Template.xlsx</t>
+    <t>Inflation</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,16 +589,16 @@
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>